<commit_message>
multi radar chart by lists
</commit_message>
<xml_diff>
--- a/test5.xlsx
+++ b/test5.xlsx
@@ -86,7 +86,271 @@
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$B$21:$B$26</f>
+              <f>'Sheet'!$C$21:$C$26</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </radarChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="2"/>
+  <chart>
+    <plotArea>
+      <radarChart>
+        <radarStyle val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$A$56:$A$61</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sheet'!$C$56:$C$61</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </radarChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="2"/>
+  <chart>
+    <plotArea>
+      <radarChart>
+        <radarStyle val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$A$91:$A$96</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sheet'!$C$91:$C$96</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </radarChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="2"/>
+  <chart>
+    <plotArea>
+      <radarChart>
+        <radarStyle val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$A$126:$A$131</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sheet'!$C$126:$C$131</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </radarChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="2"/>
+  <chart>
+    <plotArea>
+      <radarChart>
+        <radarStyle val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$A$161:$A$166</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sheet'!$C$161:$C$166</f>
             </numRef>
           </val>
         </ser>
@@ -126,9 +390,9 @@
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>4</col>
+      <col>7</col>
       <colOff>0</colOff>
-      <row>9</row>
+      <row>17</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="2700000"/>
@@ -141,6 +405,94 @@
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>52</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>87</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="3" name="Chart 3"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>122</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="4" name="Chart 4"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>157</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="5" name="Chart 5"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>

</xml_diff>